<commit_message>
update _ equipa na folha de afetacao
</commit_message>
<xml_diff>
--- a/assets/Sheet_Template.xlsx
+++ b/assets/Sheet_Template.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27602"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27616"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RodrigoPereiraSTREAM\Documents\GitHub\timesheet-streamlit\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1F2D16-6B2A-47BB-B5E9-C432915BA3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BFE28F-85D7-4D08-B525-3F2ACC545949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9468" yWindow="17172" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21180" yWindow="0" windowWidth="30525" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Equipa de projeto" sheetId="2" r:id="rId1"/>
+    <sheet name="sheet" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Equipa de projeto'!$A$1:$G$24</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="147">
   <si>
     <t>ANO 1</t>
   </si>
@@ -266,6 +270,219 @@
   </si>
   <si>
     <t>TRL 5-9</t>
+  </si>
+  <si>
+    <t>MOD-125.3</t>
+  </si>
+  <si>
+    <t>[60]</t>
+  </si>
+  <si>
+    <t>[59]</t>
+  </si>
+  <si>
+    <t>[58]</t>
+  </si>
+  <si>
+    <t>[57]</t>
+  </si>
+  <si>
+    <t>[56]</t>
+  </si>
+  <si>
+    <t>[55]</t>
+  </si>
+  <si>
+    <t>[54]</t>
+  </si>
+  <si>
+    <t>[53]</t>
+  </si>
+  <si>
+    <t>[52]</t>
+  </si>
+  <si>
+    <t>[51]</t>
+  </si>
+  <si>
+    <t>[50]</t>
+  </si>
+  <si>
+    <t>[49]</t>
+  </si>
+  <si>
+    <t>[48]</t>
+  </si>
+  <si>
+    <t>[47]</t>
+  </si>
+  <si>
+    <t>[46]</t>
+  </si>
+  <si>
+    <t>[45]</t>
+  </si>
+  <si>
+    <t>[44]</t>
+  </si>
+  <si>
+    <t>[43]</t>
+  </si>
+  <si>
+    <t>[42]</t>
+  </si>
+  <si>
+    <t>[41]</t>
+  </si>
+  <si>
+    <t>[40]</t>
+  </si>
+  <si>
+    <t>[39]</t>
+  </si>
+  <si>
+    <t>[38]</t>
+  </si>
+  <si>
+    <t>[37]</t>
+  </si>
+  <si>
+    <t>[36]</t>
+  </si>
+  <si>
+    <t>[35]</t>
+  </si>
+  <si>
+    <t>[34]</t>
+  </si>
+  <si>
+    <t>[33]</t>
+  </si>
+  <si>
+    <t>[32]</t>
+  </si>
+  <si>
+    <t>[31]</t>
+  </si>
+  <si>
+    <t>[30]</t>
+  </si>
+  <si>
+    <t>[29]</t>
+  </si>
+  <si>
+    <t>[28]</t>
+  </si>
+  <si>
+    <t>[27]</t>
+  </si>
+  <si>
+    <t>[26]</t>
+  </si>
+  <si>
+    <t>[25]</t>
+  </si>
+  <si>
+    <t>[24]</t>
+  </si>
+  <si>
+    <t>[23]</t>
+  </si>
+  <si>
+    <t>[22]</t>
+  </si>
+  <si>
+    <t>[21]</t>
+  </si>
+  <si>
+    <t>[20]</t>
+  </si>
+  <si>
+    <t>[19]</t>
+  </si>
+  <si>
+    <t>[18]</t>
+  </si>
+  <si>
+    <t>[17]</t>
+  </si>
+  <si>
+    <t>[16]</t>
+  </si>
+  <si>
+    <t>[15]</t>
+  </si>
+  <si>
+    <t>[14]</t>
+  </si>
+  <si>
+    <t>[13]</t>
+  </si>
+  <si>
+    <t>[12]</t>
+  </si>
+  <si>
+    <t>[11]</t>
+  </si>
+  <si>
+    <t>[10]</t>
+  </si>
+  <si>
+    <t>[9]</t>
+  </si>
+  <si>
+    <t>[8]</t>
+  </si>
+  <si>
+    <t>[7]</t>
+  </si>
+  <si>
+    <t>[6]</t>
+  </si>
+  <si>
+    <t>[5]</t>
+  </si>
+  <si>
+    <t>[4]</t>
+  </si>
+  <si>
+    <t>[3]</t>
+  </si>
+  <si>
+    <t>[2]</t>
+  </si>
+  <si>
+    <t>[1]</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Montante</t>
+  </si>
+  <si>
+    <t>Data de Rescisão</t>
+  </si>
+  <si>
+    <t>Data de Inicio</t>
+  </si>
+  <si>
+    <t>Genero</t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>Remuneração</t>
+  </si>
+  <si>
+    <t>Responsável</t>
+  </si>
+  <si>
+    <t>Perfil</t>
+  </si>
+  <si>
+    <t>Equipa de projeto</t>
   </si>
 </sst>
 </file>
@@ -278,7 +495,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -384,6 +601,86 @@
       <color theme="0" tint="-0.499984740745262"/>
       <name val="GalanoGrotesque-Medium"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF505050"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="GalanoGrotesque-Medium"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF505050"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="GalanoGrotesque-Medium"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="GalanoGrotesque-Medium"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="GalanoGrotesque-Medium"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="GalanoGrotesque-Medium"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="GalanoGrotesque-Medium"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF505050"/>
+      <name val="GalanoGrotesque-Medium"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="GalanoGrotesque-Medium"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Mackay"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF505050"/>
+      <name val="GalanoGrotesque-Medium"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="GalanoGrotesque-Medium"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -423,7 +720,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="59">
+  <borders count="80">
     <border>
       <left/>
       <right/>
@@ -1251,15 +1548,249 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF0070C0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF0070C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF0070C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF0070C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF0070C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF0070C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="medium">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1498,6 +2029,9 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1537,12 +2071,179 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="61" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="60" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="20" fillId="2" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="2" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="66" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="65" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="2" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="2" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="66" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="66" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="65" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="69" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="71" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="74" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="2" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
+    <cellStyle name="Moeda 2" xfId="5" xr:uid="{AF45A226-A3ED-40F6-A143-AAF7D50D508E}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="4" xr:uid="{89304678-D5B5-4CB4-A869-F688E79ADC5A}"/>
     <cellStyle name="Normal 3 63" xfId="3" xr:uid="{589F8686-52FC-4407-98A6-9EFD19CA889D}"/>
@@ -1577,6 +2278,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>121228</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>34637</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1759613" cy="581407"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A404CAFF-0199-4F92-9AA3-2E33D3BA966E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="730828" y="225137"/>
+          <a:ext cx="1759613" cy="581407"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>121228</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>34637</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1756829" cy="590932"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F5C2DA6-251C-47CA-B630-E6A561A273FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="730828" y="225137"/>
+          <a:ext cx="1756829" cy="590932"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1841,11 +2635,1353 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76C2371F-7FA2-4313-AAC8-6CAEEB3D1A18}">
+  <sheetPr>
+    <tabColor rgb="FF002060"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:P69"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" showWhiteSpace="0" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:16" ht="21" x14ac:dyDescent="0.45">
+      <c r="B1" s="158"/>
+      <c r="C1" s="158"/>
+      <c r="D1" s="157"/>
+      <c r="E1" s="157"/>
+      <c r="F1" s="157"/>
+      <c r="G1" s="157"/>
+      <c r="H1" s="157"/>
+      <c r="I1" s="157"/>
+      <c r="J1" s="157"/>
+      <c r="K1" s="157"/>
+      <c r="L1" s="157"/>
+      <c r="M1" s="157"/>
+      <c r="N1" s="157"/>
+      <c r="O1" s="157"/>
+      <c r="P1" s="157"/>
+    </row>
+    <row r="2" spans="2:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
+      <c r="J2" s="156"/>
+      <c r="K2" s="156"/>
+      <c r="L2" s="156"/>
+      <c r="M2" s="156"/>
+      <c r="N2" s="156"/>
+      <c r="O2" s="156"/>
+      <c r="P2" s="156" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="154"/>
+      <c r="C3" s="154"/>
+      <c r="D3" s="154"/>
+      <c r="E3" s="154"/>
+      <c r="F3" s="154"/>
+      <c r="G3" s="154"/>
+      <c r="H3" s="154"/>
+      <c r="I3" s="154"/>
+      <c r="J3" s="155"/>
+      <c r="K3" s="155"/>
+      <c r="L3" s="155"/>
+      <c r="M3" s="155"/>
+      <c r="N3" s="155"/>
+      <c r="O3" s="155"/>
+      <c r="P3" s="155"/>
+    </row>
+    <row r="4" spans="2:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="154"/>
+      <c r="C4" s="154"/>
+      <c r="D4" s="153"/>
+      <c r="E4" s="153"/>
+      <c r="F4" s="153"/>
+      <c r="G4" s="153"/>
+      <c r="H4" s="153"/>
+      <c r="I4" s="153"/>
+      <c r="J4" s="152"/>
+      <c r="K4" s="152"/>
+      <c r="L4" s="152"/>
+      <c r="M4" s="152"/>
+      <c r="N4" s="152"/>
+      <c r="O4" s="152"/>
+      <c r="P4" s="151"/>
+    </row>
+    <row r="6" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="150"/>
+      <c r="C6" s="149" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" s="149" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" s="149"/>
+      <c r="F6" s="149"/>
+      <c r="G6" s="149"/>
+      <c r="H6" s="148"/>
+      <c r="I6" s="149" t="s">
+        <v>143</v>
+      </c>
+      <c r="J6" s="149"/>
+      <c r="K6" s="149"/>
+      <c r="L6" s="149"/>
+      <c r="M6" s="149"/>
+      <c r="N6" s="149"/>
+      <c r="O6" s="149"/>
+      <c r="P6" s="149"/>
+    </row>
+    <row r="7" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="150"/>
+      <c r="C7" s="149"/>
+      <c r="D7" s="147"/>
+      <c r="E7" s="147"/>
+      <c r="F7" s="147"/>
+      <c r="G7" s="147"/>
+      <c r="H7" s="148"/>
+      <c r="I7" s="147"/>
+      <c r="J7" s="147"/>
+      <c r="K7" s="147"/>
+      <c r="L7" s="147"/>
+      <c r="M7" s="147"/>
+      <c r="N7" s="147"/>
+      <c r="O7" s="147"/>
+      <c r="P7" s="147"/>
+    </row>
+    <row r="8" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="146"/>
+      <c r="C8" s="145"/>
+      <c r="D8" s="143" t="s">
+        <v>142</v>
+      </c>
+      <c r="E8" s="143" t="s">
+        <v>141</v>
+      </c>
+      <c r="F8" s="143" t="s">
+        <v>140</v>
+      </c>
+      <c r="G8" s="144" t="s">
+        <v>139</v>
+      </c>
+      <c r="H8" s="143"/>
+      <c r="I8" s="143" t="s">
+        <v>138</v>
+      </c>
+      <c r="J8" s="143" t="s">
+        <v>137</v>
+      </c>
+      <c r="K8" s="143" t="s">
+        <v>138</v>
+      </c>
+      <c r="L8" s="143" t="s">
+        <v>137</v>
+      </c>
+      <c r="M8" s="143" t="s">
+        <v>138</v>
+      </c>
+      <c r="N8" s="143" t="s">
+        <v>137</v>
+      </c>
+      <c r="O8" s="143" t="s">
+        <v>138</v>
+      </c>
+      <c r="P8" s="143" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="142" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="141"/>
+      <c r="D9" s="140"/>
+      <c r="E9" s="140"/>
+      <c r="F9" s="139"/>
+      <c r="G9" s="138"/>
+      <c r="H9" s="137"/>
+      <c r="I9" s="136"/>
+      <c r="J9" s="135"/>
+      <c r="K9" s="133"/>
+      <c r="L9" s="134"/>
+      <c r="M9" s="133"/>
+      <c r="N9" s="132"/>
+      <c r="O9" s="131"/>
+      <c r="P9" s="130"/>
+    </row>
+    <row r="10" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="121" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" s="126"/>
+      <c r="D10" s="118"/>
+      <c r="E10" s="118"/>
+      <c r="F10" s="117"/>
+      <c r="G10" s="116"/>
+      <c r="H10" s="125"/>
+      <c r="I10" s="114"/>
+      <c r="J10" s="113"/>
+      <c r="K10" s="124"/>
+      <c r="L10" s="123"/>
+      <c r="M10" s="124"/>
+      <c r="N10" s="123"/>
+      <c r="O10" s="114"/>
+      <c r="P10" s="111"/>
+    </row>
+    <row r="11" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="121" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" s="126"/>
+      <c r="D11" s="118"/>
+      <c r="E11" s="129"/>
+      <c r="F11" s="117"/>
+      <c r="G11" s="116"/>
+      <c r="H11" s="125"/>
+      <c r="I11" s="114"/>
+      <c r="J11" s="113"/>
+      <c r="K11" s="124"/>
+      <c r="L11" s="123"/>
+      <c r="M11" s="124"/>
+      <c r="N11" s="123"/>
+      <c r="O11" s="114"/>
+      <c r="P11" s="111"/>
+    </row>
+    <row r="12" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="121" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" s="126"/>
+      <c r="D12" s="118"/>
+      <c r="E12" s="118"/>
+      <c r="F12" s="117"/>
+      <c r="G12" s="116"/>
+      <c r="H12" s="125"/>
+      <c r="I12" s="114"/>
+      <c r="J12" s="113"/>
+      <c r="K12" s="124"/>
+      <c r="L12" s="123"/>
+      <c r="M12" s="124"/>
+      <c r="N12" s="123"/>
+      <c r="O12" s="114"/>
+      <c r="P12" s="111"/>
+    </row>
+    <row r="13" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="121" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="126"/>
+      <c r="D13" s="118"/>
+      <c r="E13" s="118"/>
+      <c r="F13" s="117"/>
+      <c r="G13" s="127"/>
+      <c r="H13" s="125"/>
+      <c r="I13" s="114"/>
+      <c r="J13" s="113"/>
+      <c r="K13" s="128"/>
+      <c r="L13" s="123"/>
+      <c r="M13" s="124"/>
+      <c r="N13" s="123"/>
+      <c r="O13" s="114"/>
+      <c r="P13" s="111"/>
+    </row>
+    <row r="14" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="121" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" s="126"/>
+      <c r="D14" s="118"/>
+      <c r="E14" s="118"/>
+      <c r="F14" s="117"/>
+      <c r="G14" s="116"/>
+      <c r="H14" s="125"/>
+      <c r="I14" s="114"/>
+      <c r="J14" s="113"/>
+      <c r="K14" s="128"/>
+      <c r="L14" s="123"/>
+      <c r="M14" s="124"/>
+      <c r="N14" s="123"/>
+      <c r="O14" s="114"/>
+      <c r="P14" s="111"/>
+    </row>
+    <row r="15" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="121" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="120"/>
+      <c r="D15" s="118"/>
+      <c r="E15" s="118"/>
+      <c r="F15" s="117"/>
+      <c r="G15" s="127"/>
+      <c r="H15" s="125"/>
+      <c r="I15" s="114"/>
+      <c r="J15" s="113"/>
+      <c r="K15" s="124"/>
+      <c r="L15" s="123"/>
+      <c r="M15" s="124"/>
+      <c r="N15" s="123"/>
+      <c r="O15" s="114"/>
+      <c r="P15" s="111"/>
+    </row>
+    <row r="16" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="121" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" s="126"/>
+      <c r="D16" s="118"/>
+      <c r="E16" s="118"/>
+      <c r="F16" s="117"/>
+      <c r="G16" s="116"/>
+      <c r="H16" s="125"/>
+      <c r="I16" s="114"/>
+      <c r="J16" s="113"/>
+      <c r="K16" s="124"/>
+      <c r="L16" s="123"/>
+      <c r="M16" s="124"/>
+      <c r="N16" s="123"/>
+      <c r="O16" s="114"/>
+      <c r="P16" s="111"/>
+    </row>
+    <row r="17" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="121" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" s="120"/>
+      <c r="D17" s="118"/>
+      <c r="E17" s="118"/>
+      <c r="F17" s="117"/>
+      <c r="G17" s="116"/>
+      <c r="H17" s="125"/>
+      <c r="I17" s="114"/>
+      <c r="J17" s="113"/>
+      <c r="K17" s="124"/>
+      <c r="L17" s="123"/>
+      <c r="M17" s="124"/>
+      <c r="N17" s="123"/>
+      <c r="O17" s="114"/>
+      <c r="P17" s="111"/>
+    </row>
+    <row r="18" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="121" t="s">
+        <v>127</v>
+      </c>
+      <c r="C18" s="120"/>
+      <c r="D18" s="118"/>
+      <c r="E18" s="118"/>
+      <c r="F18" s="117"/>
+      <c r="G18" s="116"/>
+      <c r="H18" s="125"/>
+      <c r="I18" s="114"/>
+      <c r="J18" s="113"/>
+      <c r="K18" s="124"/>
+      <c r="L18" s="123"/>
+      <c r="M18" s="124"/>
+      <c r="N18" s="123"/>
+      <c r="O18" s="114"/>
+      <c r="P18" s="111"/>
+    </row>
+    <row r="19" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="121" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19" s="120"/>
+      <c r="D19" s="118"/>
+      <c r="E19" s="118"/>
+      <c r="F19" s="117"/>
+      <c r="G19" s="116"/>
+      <c r="H19" s="125"/>
+      <c r="I19" s="114"/>
+      <c r="J19" s="113"/>
+      <c r="K19" s="124"/>
+      <c r="L19" s="123"/>
+      <c r="M19" s="124"/>
+      <c r="N19" s="123"/>
+      <c r="O19" s="114"/>
+      <c r="P19" s="111"/>
+    </row>
+    <row r="20" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="121" t="s">
+        <v>125</v>
+      </c>
+      <c r="C20" s="120"/>
+      <c r="D20" s="118"/>
+      <c r="E20" s="118"/>
+      <c r="F20" s="117"/>
+      <c r="G20" s="116"/>
+      <c r="H20" s="125"/>
+      <c r="I20" s="114"/>
+      <c r="J20" s="113"/>
+      <c r="K20" s="124"/>
+      <c r="L20" s="123"/>
+      <c r="M20" s="124"/>
+      <c r="N20" s="123"/>
+      <c r="O20" s="114"/>
+      <c r="P20" s="111"/>
+    </row>
+    <row r="21" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="121" t="s">
+        <v>124</v>
+      </c>
+      <c r="C21" s="120"/>
+      <c r="D21" s="118"/>
+      <c r="E21" s="118"/>
+      <c r="F21" s="117"/>
+      <c r="G21" s="116"/>
+      <c r="H21" s="125"/>
+      <c r="I21" s="114"/>
+      <c r="J21" s="113"/>
+      <c r="K21" s="124"/>
+      <c r="L21" s="123"/>
+      <c r="M21" s="124"/>
+      <c r="N21" s="123"/>
+      <c r="O21" s="114"/>
+      <c r="P21" s="111"/>
+    </row>
+    <row r="22" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="121" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" s="120"/>
+      <c r="D22" s="118"/>
+      <c r="E22" s="118"/>
+      <c r="F22" s="117"/>
+      <c r="G22" s="116"/>
+      <c r="H22" s="115"/>
+      <c r="I22" s="114"/>
+      <c r="J22" s="113"/>
+      <c r="K22" s="112"/>
+      <c r="L22" s="113"/>
+      <c r="M22" s="112"/>
+      <c r="N22" s="113"/>
+      <c r="O22" s="112"/>
+      <c r="P22" s="111"/>
+    </row>
+    <row r="23" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="121" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" s="120"/>
+      <c r="D23" s="118"/>
+      <c r="E23" s="118"/>
+      <c r="F23" s="117"/>
+      <c r="G23" s="116"/>
+      <c r="H23" s="115"/>
+      <c r="I23" s="114"/>
+      <c r="J23" s="113"/>
+      <c r="K23" s="112"/>
+      <c r="L23" s="113"/>
+      <c r="M23" s="112"/>
+      <c r="N23" s="113"/>
+      <c r="O23" s="112"/>
+      <c r="P23" s="111"/>
+    </row>
+    <row r="24" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="121" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" s="120"/>
+      <c r="D24" s="118"/>
+      <c r="E24" s="118"/>
+      <c r="F24" s="117"/>
+      <c r="G24" s="116"/>
+      <c r="H24" s="115"/>
+      <c r="I24" s="114"/>
+      <c r="J24" s="113"/>
+      <c r="K24" s="112"/>
+      <c r="L24" s="113"/>
+      <c r="M24" s="112"/>
+      <c r="N24" s="113"/>
+      <c r="O24" s="112"/>
+      <c r="P24" s="111"/>
+    </row>
+    <row r="25" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="121" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="120"/>
+      <c r="D25" s="118"/>
+      <c r="E25" s="118"/>
+      <c r="F25" s="117"/>
+      <c r="G25" s="116"/>
+      <c r="H25" s="115"/>
+      <c r="I25" s="114"/>
+      <c r="J25" s="113"/>
+      <c r="K25" s="112"/>
+      <c r="L25" s="113"/>
+      <c r="M25" s="112"/>
+      <c r="N25" s="113"/>
+      <c r="O25" s="112"/>
+      <c r="P25" s="111"/>
+    </row>
+    <row r="26" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="121" t="s">
+        <v>119</v>
+      </c>
+      <c r="C26" s="120"/>
+      <c r="D26" s="118"/>
+      <c r="E26" s="118"/>
+      <c r="F26" s="117"/>
+      <c r="G26" s="116"/>
+      <c r="H26" s="115"/>
+      <c r="I26" s="114"/>
+      <c r="J26" s="113"/>
+      <c r="K26" s="112"/>
+      <c r="L26" s="113"/>
+      <c r="M26" s="112"/>
+      <c r="N26" s="113"/>
+      <c r="O26" s="112"/>
+      <c r="P26" s="111"/>
+    </row>
+    <row r="27" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="121" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" s="120"/>
+      <c r="D27" s="118"/>
+      <c r="E27" s="118"/>
+      <c r="F27" s="117"/>
+      <c r="G27" s="116"/>
+      <c r="H27" s="115"/>
+      <c r="I27" s="114"/>
+      <c r="J27" s="113"/>
+      <c r="K27" s="112"/>
+      <c r="L27" s="113"/>
+      <c r="M27" s="112"/>
+      <c r="N27" s="113"/>
+      <c r="O27" s="112"/>
+      <c r="P27" s="111"/>
+    </row>
+    <row r="28" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="121" t="s">
+        <v>117</v>
+      </c>
+      <c r="C28" s="120"/>
+      <c r="D28" s="118"/>
+      <c r="E28" s="118"/>
+      <c r="F28" s="117"/>
+      <c r="G28" s="116"/>
+      <c r="H28" s="115"/>
+      <c r="I28" s="114"/>
+      <c r="J28" s="113"/>
+      <c r="K28" s="112"/>
+      <c r="L28" s="113"/>
+      <c r="M28" s="112"/>
+      <c r="N28" s="113"/>
+      <c r="O28" s="112"/>
+      <c r="P28" s="111"/>
+    </row>
+    <row r="29" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="121" t="s">
+        <v>116</v>
+      </c>
+      <c r="C29" s="120"/>
+      <c r="D29" s="118"/>
+      <c r="E29" s="118"/>
+      <c r="F29" s="117"/>
+      <c r="G29" s="116"/>
+      <c r="H29" s="115"/>
+      <c r="I29" s="114"/>
+      <c r="J29" s="113"/>
+      <c r="K29" s="112"/>
+      <c r="L29" s="113"/>
+      <c r="M29" s="112"/>
+      <c r="N29" s="113"/>
+      <c r="O29" s="112"/>
+      <c r="P29" s="111"/>
+    </row>
+    <row r="30" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="121" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" s="120"/>
+      <c r="D30" s="118"/>
+      <c r="E30" s="118"/>
+      <c r="F30" s="117"/>
+      <c r="G30" s="116"/>
+      <c r="H30" s="115"/>
+      <c r="I30" s="114"/>
+      <c r="J30" s="113"/>
+      <c r="K30" s="112"/>
+      <c r="L30" s="113"/>
+      <c r="M30" s="112"/>
+      <c r="N30" s="113"/>
+      <c r="O30" s="112"/>
+      <c r="P30" s="111"/>
+    </row>
+    <row r="31" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="121" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31" s="120"/>
+      <c r="D31" s="118"/>
+      <c r="E31" s="118"/>
+      <c r="F31" s="117"/>
+      <c r="G31" s="116"/>
+      <c r="H31" s="115"/>
+      <c r="I31" s="114"/>
+      <c r="J31" s="113"/>
+      <c r="K31" s="112"/>
+      <c r="L31" s="113"/>
+      <c r="M31" s="112"/>
+      <c r="N31" s="113"/>
+      <c r="O31" s="112"/>
+      <c r="P31" s="111"/>
+    </row>
+    <row r="32" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="121" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32" s="120"/>
+      <c r="D32" s="118"/>
+      <c r="E32" s="118"/>
+      <c r="F32" s="117"/>
+      <c r="G32" s="116"/>
+      <c r="H32" s="115"/>
+      <c r="I32" s="114"/>
+      <c r="J32" s="113"/>
+      <c r="K32" s="112"/>
+      <c r="L32" s="113"/>
+      <c r="M32" s="112"/>
+      <c r="N32" s="113"/>
+      <c r="O32" s="112"/>
+      <c r="P32" s="111"/>
+    </row>
+    <row r="33" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="121" t="s">
+        <v>112</v>
+      </c>
+      <c r="C33" s="120"/>
+      <c r="D33" s="118"/>
+      <c r="E33" s="118"/>
+      <c r="F33" s="117"/>
+      <c r="G33" s="116"/>
+      <c r="H33" s="115"/>
+      <c r="I33" s="114"/>
+      <c r="J33" s="113"/>
+      <c r="K33" s="112"/>
+      <c r="L33" s="113"/>
+      <c r="M33" s="112"/>
+      <c r="N33" s="113"/>
+      <c r="O33" s="112"/>
+      <c r="P33" s="111"/>
+    </row>
+    <row r="34" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="121" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="120"/>
+      <c r="D34" s="118"/>
+      <c r="E34" s="118"/>
+      <c r="F34" s="117"/>
+      <c r="G34" s="116"/>
+      <c r="H34" s="115"/>
+      <c r="I34" s="114"/>
+      <c r="J34" s="113"/>
+      <c r="K34" s="112"/>
+      <c r="L34" s="113"/>
+      <c r="M34" s="112"/>
+      <c r="N34" s="113"/>
+      <c r="O34" s="112"/>
+      <c r="P34" s="111"/>
+    </row>
+    <row r="35" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="121" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" s="120"/>
+      <c r="D35" s="118"/>
+      <c r="E35" s="118"/>
+      <c r="F35" s="117"/>
+      <c r="G35" s="116"/>
+      <c r="H35" s="115"/>
+      <c r="I35" s="114"/>
+      <c r="J35" s="113"/>
+      <c r="K35" s="112"/>
+      <c r="L35" s="113"/>
+      <c r="M35" s="112"/>
+      <c r="N35" s="113"/>
+      <c r="O35" s="112"/>
+      <c r="P35" s="111"/>
+    </row>
+    <row r="36" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="121" t="s">
+        <v>109</v>
+      </c>
+      <c r="C36" s="120"/>
+      <c r="D36" s="118"/>
+      <c r="E36" s="118"/>
+      <c r="F36" s="117"/>
+      <c r="G36" s="116"/>
+      <c r="H36" s="115"/>
+      <c r="I36" s="114"/>
+      <c r="J36" s="113"/>
+      <c r="K36" s="112"/>
+      <c r="L36" s="113"/>
+      <c r="M36" s="112"/>
+      <c r="N36" s="113"/>
+      <c r="O36" s="112"/>
+      <c r="P36" s="111"/>
+    </row>
+    <row r="37" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="121" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="120"/>
+      <c r="D37" s="118"/>
+      <c r="E37" s="118"/>
+      <c r="F37" s="117"/>
+      <c r="G37" s="116"/>
+      <c r="H37" s="115"/>
+      <c r="I37" s="114"/>
+      <c r="J37" s="113"/>
+      <c r="K37" s="112"/>
+      <c r="L37" s="113"/>
+      <c r="M37" s="112"/>
+      <c r="N37" s="113"/>
+      <c r="O37" s="112"/>
+      <c r="P37" s="111"/>
+    </row>
+    <row r="38" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="121" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" s="120"/>
+      <c r="D38" s="118"/>
+      <c r="E38" s="118"/>
+      <c r="F38" s="117"/>
+      <c r="G38" s="116"/>
+      <c r="H38" s="115"/>
+      <c r="I38" s="114"/>
+      <c r="J38" s="113"/>
+      <c r="K38" s="112"/>
+      <c r="L38" s="113"/>
+      <c r="M38" s="112"/>
+      <c r="N38" s="113"/>
+      <c r="O38" s="112"/>
+      <c r="P38" s="111"/>
+    </row>
+    <row r="39" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="121" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39" s="120"/>
+      <c r="D39" s="118"/>
+      <c r="E39" s="118"/>
+      <c r="F39" s="117"/>
+      <c r="G39" s="116"/>
+      <c r="H39" s="115"/>
+      <c r="I39" s="114"/>
+      <c r="J39" s="113"/>
+      <c r="K39" s="112"/>
+      <c r="L39" s="113"/>
+      <c r="M39" s="112"/>
+      <c r="N39" s="113"/>
+      <c r="O39" s="112"/>
+      <c r="P39" s="111"/>
+    </row>
+    <row r="40" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="121" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="120"/>
+      <c r="D40" s="118"/>
+      <c r="E40" s="118"/>
+      <c r="F40" s="117"/>
+      <c r="G40" s="116"/>
+      <c r="H40" s="115"/>
+      <c r="I40" s="114"/>
+      <c r="J40" s="113"/>
+      <c r="K40" s="112"/>
+      <c r="L40" s="113"/>
+      <c r="M40" s="112"/>
+      <c r="N40" s="113"/>
+      <c r="O40" s="112"/>
+      <c r="P40" s="111"/>
+    </row>
+    <row r="41" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="121" t="s">
+        <v>104</v>
+      </c>
+      <c r="C41" s="120"/>
+      <c r="D41" s="118"/>
+      <c r="E41" s="118"/>
+      <c r="F41" s="117"/>
+      <c r="G41" s="116"/>
+      <c r="H41" s="115"/>
+      <c r="I41" s="114"/>
+      <c r="J41" s="113"/>
+      <c r="K41" s="112"/>
+      <c r="L41" s="113"/>
+      <c r="M41" s="112"/>
+      <c r="N41" s="113"/>
+      <c r="O41" s="112"/>
+      <c r="P41" s="111"/>
+    </row>
+    <row r="42" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="121" t="s">
+        <v>103</v>
+      </c>
+      <c r="C42" s="120"/>
+      <c r="D42" s="119"/>
+      <c r="E42" s="118"/>
+      <c r="F42" s="117"/>
+      <c r="G42" s="116"/>
+      <c r="H42" s="115"/>
+      <c r="I42" s="114"/>
+      <c r="J42" s="113"/>
+      <c r="K42" s="112"/>
+      <c r="L42" s="113"/>
+      <c r="M42" s="122"/>
+      <c r="N42" s="113"/>
+      <c r="O42" s="112"/>
+      <c r="P42" s="111"/>
+    </row>
+    <row r="43" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="121" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43" s="120"/>
+      <c r="D43" s="119"/>
+      <c r="E43" s="118"/>
+      <c r="F43" s="117"/>
+      <c r="G43" s="116"/>
+      <c r="H43" s="115"/>
+      <c r="I43" s="114"/>
+      <c r="J43" s="113"/>
+      <c r="K43" s="112"/>
+      <c r="L43" s="113"/>
+      <c r="M43" s="112"/>
+      <c r="N43" s="113"/>
+      <c r="O43" s="112"/>
+      <c r="P43" s="111"/>
+    </row>
+    <row r="44" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="121" t="s">
+        <v>101</v>
+      </c>
+      <c r="C44" s="120"/>
+      <c r="D44" s="119"/>
+      <c r="E44" s="118"/>
+      <c r="F44" s="117"/>
+      <c r="G44" s="116"/>
+      <c r="H44" s="115"/>
+      <c r="I44" s="114"/>
+      <c r="J44" s="113"/>
+      <c r="K44" s="112"/>
+      <c r="L44" s="113"/>
+      <c r="M44" s="112"/>
+      <c r="N44" s="113"/>
+      <c r="O44" s="112"/>
+      <c r="P44" s="111"/>
+    </row>
+    <row r="45" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="121" t="s">
+        <v>100</v>
+      </c>
+      <c r="C45" s="120"/>
+      <c r="D45" s="119"/>
+      <c r="E45" s="118"/>
+      <c r="F45" s="117"/>
+      <c r="G45" s="116"/>
+      <c r="H45" s="115"/>
+      <c r="I45" s="114"/>
+      <c r="J45" s="113"/>
+      <c r="K45" s="112"/>
+      <c r="L45" s="113"/>
+      <c r="M45" s="112"/>
+      <c r="N45" s="113"/>
+      <c r="O45" s="112"/>
+      <c r="P45" s="111"/>
+    </row>
+    <row r="46" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="121" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46" s="120"/>
+      <c r="D46" s="119"/>
+      <c r="E46" s="118"/>
+      <c r="F46" s="117"/>
+      <c r="G46" s="116"/>
+      <c r="H46" s="115"/>
+      <c r="I46" s="114"/>
+      <c r="J46" s="113"/>
+      <c r="K46" s="112"/>
+      <c r="L46" s="113"/>
+      <c r="M46" s="112"/>
+      <c r="N46" s="113"/>
+      <c r="O46" s="112"/>
+      <c r="P46" s="111"/>
+    </row>
+    <row r="47" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="121" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" s="120"/>
+      <c r="D47" s="119"/>
+      <c r="E47" s="118"/>
+      <c r="F47" s="117"/>
+      <c r="G47" s="116"/>
+      <c r="H47" s="115"/>
+      <c r="I47" s="114"/>
+      <c r="J47" s="113"/>
+      <c r="K47" s="112"/>
+      <c r="L47" s="113"/>
+      <c r="M47" s="112"/>
+      <c r="N47" s="113"/>
+      <c r="O47" s="112"/>
+      <c r="P47" s="111"/>
+    </row>
+    <row r="48" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="121" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" s="120"/>
+      <c r="D48" s="119"/>
+      <c r="E48" s="118"/>
+      <c r="F48" s="117"/>
+      <c r="G48" s="116"/>
+      <c r="H48" s="115"/>
+      <c r="I48" s="114"/>
+      <c r="J48" s="113"/>
+      <c r="K48" s="112"/>
+      <c r="L48" s="113"/>
+      <c r="M48" s="112"/>
+      <c r="N48" s="113"/>
+      <c r="O48" s="112"/>
+      <c r="P48" s="111"/>
+    </row>
+    <row r="49" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="121" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" s="120"/>
+      <c r="D49" s="119"/>
+      <c r="E49" s="118"/>
+      <c r="F49" s="117"/>
+      <c r="G49" s="116"/>
+      <c r="H49" s="115"/>
+      <c r="I49" s="114"/>
+      <c r="J49" s="113"/>
+      <c r="K49" s="112"/>
+      <c r="L49" s="113"/>
+      <c r="M49" s="122"/>
+      <c r="N49" s="113"/>
+      <c r="O49" s="112"/>
+      <c r="P49" s="111"/>
+    </row>
+    <row r="50" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="121" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" s="120"/>
+      <c r="D50" s="119"/>
+      <c r="E50" s="118"/>
+      <c r="F50" s="117"/>
+      <c r="G50" s="116"/>
+      <c r="H50" s="115"/>
+      <c r="I50" s="114"/>
+      <c r="J50" s="113"/>
+      <c r="K50" s="112"/>
+      <c r="L50" s="113"/>
+      <c r="M50" s="112"/>
+      <c r="N50" s="113"/>
+      <c r="O50" s="112"/>
+      <c r="P50" s="111"/>
+    </row>
+    <row r="51" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="121" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" s="120"/>
+      <c r="D51" s="119"/>
+      <c r="E51" s="118"/>
+      <c r="F51" s="117"/>
+      <c r="G51" s="116"/>
+      <c r="H51" s="115"/>
+      <c r="I51" s="114"/>
+      <c r="J51" s="113"/>
+      <c r="K51" s="112"/>
+      <c r="L51" s="113"/>
+      <c r="M51" s="122"/>
+      <c r="N51" s="113"/>
+      <c r="O51" s="112"/>
+      <c r="P51" s="111"/>
+    </row>
+    <row r="52" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="121" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52" s="120"/>
+      <c r="D52" s="119"/>
+      <c r="E52" s="118"/>
+      <c r="F52" s="117"/>
+      <c r="G52" s="116"/>
+      <c r="H52" s="115"/>
+      <c r="I52" s="114"/>
+      <c r="J52" s="113"/>
+      <c r="K52" s="112"/>
+      <c r="L52" s="113"/>
+      <c r="M52" s="112"/>
+      <c r="N52" s="113"/>
+      <c r="O52" s="112"/>
+      <c r="P52" s="111"/>
+    </row>
+    <row r="53" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="121" t="s">
+        <v>92</v>
+      </c>
+      <c r="C53" s="120"/>
+      <c r="D53" s="119"/>
+      <c r="E53" s="118"/>
+      <c r="F53" s="117"/>
+      <c r="G53" s="116"/>
+      <c r="H53" s="115"/>
+      <c r="I53" s="114"/>
+      <c r="J53" s="113"/>
+      <c r="K53" s="112"/>
+      <c r="L53" s="113"/>
+      <c r="M53" s="112"/>
+      <c r="N53" s="113"/>
+      <c r="O53" s="112"/>
+      <c r="P53" s="111"/>
+    </row>
+    <row r="54" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="121" t="s">
+        <v>91</v>
+      </c>
+      <c r="C54" s="120"/>
+      <c r="D54" s="119"/>
+      <c r="E54" s="118"/>
+      <c r="F54" s="117"/>
+      <c r="G54" s="116"/>
+      <c r="H54" s="115"/>
+      <c r="I54" s="114"/>
+      <c r="J54" s="113"/>
+      <c r="K54" s="112"/>
+      <c r="L54" s="113"/>
+      <c r="M54" s="112"/>
+      <c r="N54" s="113"/>
+      <c r="O54" s="112"/>
+      <c r="P54" s="111"/>
+    </row>
+    <row r="55" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="121" t="s">
+        <v>90</v>
+      </c>
+      <c r="C55" s="120"/>
+      <c r="D55" s="117"/>
+      <c r="E55" s="118"/>
+      <c r="F55" s="117"/>
+      <c r="G55" s="116"/>
+      <c r="H55" s="115"/>
+      <c r="I55" s="114"/>
+      <c r="J55" s="113"/>
+      <c r="K55" s="112"/>
+      <c r="L55" s="113"/>
+      <c r="M55" s="112"/>
+      <c r="N55" s="113"/>
+      <c r="O55" s="112"/>
+      <c r="P55" s="111"/>
+    </row>
+    <row r="56" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="121" t="s">
+        <v>89</v>
+      </c>
+      <c r="C56" s="120"/>
+      <c r="D56" s="119"/>
+      <c r="E56" s="118"/>
+      <c r="F56" s="117"/>
+      <c r="G56" s="116"/>
+      <c r="H56" s="115"/>
+      <c r="I56" s="114"/>
+      <c r="J56" s="113"/>
+      <c r="K56" s="112"/>
+      <c r="L56" s="113"/>
+      <c r="M56" s="112"/>
+      <c r="N56" s="113"/>
+      <c r="O56" s="112"/>
+      <c r="P56" s="111"/>
+    </row>
+    <row r="57" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="121" t="s">
+        <v>88</v>
+      </c>
+      <c r="C57" s="120"/>
+      <c r="D57" s="119"/>
+      <c r="E57" s="118"/>
+      <c r="F57" s="117"/>
+      <c r="G57" s="116"/>
+      <c r="H57" s="115"/>
+      <c r="I57" s="114"/>
+      <c r="J57" s="113"/>
+      <c r="K57" s="112"/>
+      <c r="L57" s="113"/>
+      <c r="M57" s="112"/>
+      <c r="N57" s="113"/>
+      <c r="O57" s="112"/>
+      <c r="P57" s="111"/>
+    </row>
+    <row r="58" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="121" t="s">
+        <v>87</v>
+      </c>
+      <c r="C58" s="120"/>
+      <c r="D58" s="119"/>
+      <c r="E58" s="118"/>
+      <c r="F58" s="117"/>
+      <c r="G58" s="116"/>
+      <c r="H58" s="115"/>
+      <c r="I58" s="114"/>
+      <c r="J58" s="113"/>
+      <c r="K58" s="112"/>
+      <c r="L58" s="113"/>
+      <c r="M58" s="112"/>
+      <c r="N58" s="113"/>
+      <c r="O58" s="112"/>
+      <c r="P58" s="111"/>
+    </row>
+    <row r="59" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="121" t="s">
+        <v>86</v>
+      </c>
+      <c r="C59" s="120"/>
+      <c r="D59" s="119"/>
+      <c r="E59" s="118"/>
+      <c r="F59" s="117"/>
+      <c r="G59" s="116"/>
+      <c r="H59" s="115"/>
+      <c r="I59" s="114"/>
+      <c r="J59" s="113"/>
+      <c r="K59" s="112"/>
+      <c r="L59" s="113"/>
+      <c r="M59" s="112"/>
+      <c r="N59" s="113"/>
+      <c r="O59" s="112"/>
+      <c r="P59" s="111"/>
+    </row>
+    <row r="60" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="121" t="s">
+        <v>85</v>
+      </c>
+      <c r="C60" s="120"/>
+      <c r="D60" s="119"/>
+      <c r="E60" s="118"/>
+      <c r="F60" s="117"/>
+      <c r="G60" s="116"/>
+      <c r="H60" s="115"/>
+      <c r="I60" s="114"/>
+      <c r="J60" s="113"/>
+      <c r="K60" s="112"/>
+      <c r="L60" s="113"/>
+      <c r="M60" s="112"/>
+      <c r="N60" s="113"/>
+      <c r="O60" s="112"/>
+      <c r="P60" s="111"/>
+    </row>
+    <row r="61" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="121" t="s">
+        <v>84</v>
+      </c>
+      <c r="C61" s="120"/>
+      <c r="D61" s="119"/>
+      <c r="E61" s="118"/>
+      <c r="F61" s="117"/>
+      <c r="G61" s="116"/>
+      <c r="H61" s="115"/>
+      <c r="I61" s="114"/>
+      <c r="J61" s="113"/>
+      <c r="K61" s="112"/>
+      <c r="L61" s="113"/>
+      <c r="M61" s="112"/>
+      <c r="N61" s="113"/>
+      <c r="O61" s="112"/>
+      <c r="P61" s="111"/>
+    </row>
+    <row r="62" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="121" t="s">
+        <v>83</v>
+      </c>
+      <c r="C62" s="120"/>
+      <c r="D62" s="119"/>
+      <c r="E62" s="118"/>
+      <c r="F62" s="117"/>
+      <c r="G62" s="116"/>
+      <c r="H62" s="115"/>
+      <c r="I62" s="114"/>
+      <c r="J62" s="113"/>
+      <c r="K62" s="112"/>
+      <c r="L62" s="113"/>
+      <c r="M62" s="112"/>
+      <c r="N62" s="113"/>
+      <c r="O62" s="112"/>
+      <c r="P62" s="111"/>
+    </row>
+    <row r="63" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="121" t="s">
+        <v>82</v>
+      </c>
+      <c r="C63" s="120"/>
+      <c r="D63" s="119"/>
+      <c r="E63" s="118"/>
+      <c r="F63" s="117"/>
+      <c r="G63" s="116"/>
+      <c r="H63" s="115"/>
+      <c r="I63" s="114"/>
+      <c r="J63" s="113"/>
+      <c r="K63" s="112"/>
+      <c r="L63" s="113"/>
+      <c r="M63" s="112"/>
+      <c r="N63" s="113"/>
+      <c r="O63" s="112"/>
+      <c r="P63" s="111"/>
+    </row>
+    <row r="64" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="121" t="s">
+        <v>81</v>
+      </c>
+      <c r="C64" s="120"/>
+      <c r="D64" s="119"/>
+      <c r="E64" s="118"/>
+      <c r="F64" s="117"/>
+      <c r="G64" s="116"/>
+      <c r="H64" s="115"/>
+      <c r="I64" s="114"/>
+      <c r="J64" s="113"/>
+      <c r="K64" s="112"/>
+      <c r="L64" s="113"/>
+      <c r="M64" s="112"/>
+      <c r="N64" s="113"/>
+      <c r="O64" s="112"/>
+      <c r="P64" s="111"/>
+    </row>
+    <row r="65" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="121" t="s">
+        <v>80</v>
+      </c>
+      <c r="C65" s="120"/>
+      <c r="D65" s="119"/>
+      <c r="E65" s="118"/>
+      <c r="F65" s="117"/>
+      <c r="G65" s="116"/>
+      <c r="H65" s="115"/>
+      <c r="I65" s="114"/>
+      <c r="J65" s="113"/>
+      <c r="K65" s="112"/>
+      <c r="L65" s="113"/>
+      <c r="M65" s="122"/>
+      <c r="N65" s="113"/>
+      <c r="O65" s="112"/>
+      <c r="P65" s="111"/>
+    </row>
+    <row r="66" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="121" t="s">
+        <v>79</v>
+      </c>
+      <c r="C66" s="120"/>
+      <c r="D66" s="119"/>
+      <c r="E66" s="118"/>
+      <c r="F66" s="117"/>
+      <c r="G66" s="116"/>
+      <c r="H66" s="115"/>
+      <c r="I66" s="114"/>
+      <c r="J66" s="113"/>
+      <c r="K66" s="112"/>
+      <c r="L66" s="113"/>
+      <c r="M66" s="122"/>
+      <c r="N66" s="113"/>
+      <c r="O66" s="112"/>
+      <c r="P66" s="111"/>
+    </row>
+    <row r="67" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="121" t="s">
+        <v>78</v>
+      </c>
+      <c r="C67" s="120"/>
+      <c r="D67" s="119"/>
+      <c r="E67" s="118"/>
+      <c r="F67" s="117"/>
+      <c r="G67" s="116"/>
+      <c r="H67" s="115"/>
+      <c r="I67" s="114"/>
+      <c r="J67" s="113"/>
+      <c r="K67" s="112"/>
+      <c r="L67" s="113"/>
+      <c r="M67" s="112"/>
+      <c r="N67" s="113"/>
+      <c r="O67" s="112"/>
+      <c r="P67" s="111"/>
+    </row>
+    <row r="68" spans="2:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B68" s="110" t="s">
+        <v>77</v>
+      </c>
+      <c r="C68" s="109"/>
+      <c r="D68" s="108"/>
+      <c r="E68" s="107"/>
+      <c r="F68" s="106"/>
+      <c r="G68" s="105"/>
+      <c r="H68" s="105"/>
+      <c r="I68" s="104"/>
+      <c r="J68" s="103"/>
+      <c r="K68" s="102"/>
+      <c r="L68" s="103"/>
+      <c r="M68" s="102"/>
+      <c r="N68" s="103"/>
+      <c r="O68" s="102"/>
+      <c r="P68" s="101"/>
+    </row>
+    <row r="69" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="P69" s="100" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:G7"/>
+    <mergeCell ref="I6:P7"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="41" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BL57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1887,85 +4023,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:64" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="99"/>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
+      <c r="A1" s="86"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
     </row>
     <row r="2" spans="1:64" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="93" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="94"/>
-      <c r="L2" s="94"/>
-      <c r="M2" s="94"/>
-      <c r="N2" s="94"/>
-      <c r="O2" s="94"/>
-      <c r="P2" s="95"/>
-      <c r="Q2" s="96" t="s">
+      <c r="E2" s="94" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
+      <c r="O2" s="95"/>
+      <c r="P2" s="96"/>
+      <c r="Q2" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="R2" s="97"/>
-      <c r="S2" s="97"/>
-      <c r="T2" s="97"/>
-      <c r="U2" s="97"/>
-      <c r="V2" s="97"/>
-      <c r="W2" s="97"/>
-      <c r="X2" s="97"/>
-      <c r="Y2" s="97"/>
-      <c r="Z2" s="97"/>
-      <c r="AA2" s="97"/>
-      <c r="AB2" s="98"/>
-      <c r="AC2" s="86" t="s">
+      <c r="R2" s="98"/>
+      <c r="S2" s="98"/>
+      <c r="T2" s="98"/>
+      <c r="U2" s="98"/>
+      <c r="V2" s="98"/>
+      <c r="W2" s="98"/>
+      <c r="X2" s="98"/>
+      <c r="Y2" s="98"/>
+      <c r="Z2" s="98"/>
+      <c r="AA2" s="98"/>
+      <c r="AB2" s="99"/>
+      <c r="AC2" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="AD2" s="87"/>
-      <c r="AE2" s="87"/>
-      <c r="AF2" s="87"/>
-      <c r="AG2" s="87"/>
-      <c r="AH2" s="87"/>
-      <c r="AI2" s="87"/>
-      <c r="AJ2" s="87"/>
-      <c r="AK2" s="87"/>
-      <c r="AL2" s="87"/>
-      <c r="AM2" s="87"/>
-      <c r="AN2" s="88"/>
-      <c r="AO2" s="86" t="s">
+      <c r="AD2" s="88"/>
+      <c r="AE2" s="88"/>
+      <c r="AF2" s="88"/>
+      <c r="AG2" s="88"/>
+      <c r="AH2" s="88"/>
+      <c r="AI2" s="88"/>
+      <c r="AJ2" s="88"/>
+      <c r="AK2" s="88"/>
+      <c r="AL2" s="88"/>
+      <c r="AM2" s="88"/>
+      <c r="AN2" s="89"/>
+      <c r="AO2" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="AP2" s="87"/>
-      <c r="AQ2" s="87"/>
-      <c r="AR2" s="87"/>
-      <c r="AS2" s="87"/>
-      <c r="AT2" s="87"/>
-      <c r="AU2" s="87"/>
-      <c r="AV2" s="87"/>
-      <c r="AW2" s="87"/>
-      <c r="AX2" s="87"/>
-      <c r="AY2" s="87"/>
-      <c r="AZ2" s="88"/>
-      <c r="BA2" s="86" t="s">
+      <c r="AP2" s="88"/>
+      <c r="AQ2" s="88"/>
+      <c r="AR2" s="88"/>
+      <c r="AS2" s="88"/>
+      <c r="AT2" s="88"/>
+      <c r="AU2" s="88"/>
+      <c r="AV2" s="88"/>
+      <c r="AW2" s="88"/>
+      <c r="AX2" s="88"/>
+      <c r="AY2" s="88"/>
+      <c r="AZ2" s="89"/>
+      <c r="BA2" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="BB2" s="87"/>
-      <c r="BC2" s="87"/>
-      <c r="BD2" s="87"/>
-      <c r="BE2" s="87"/>
-      <c r="BF2" s="87"/>
-      <c r="BG2" s="87"/>
-      <c r="BH2" s="87"/>
-      <c r="BI2" s="87"/>
-      <c r="BJ2" s="87"/>
-      <c r="BK2" s="87"/>
-      <c r="BL2" s="88"/>
+      <c r="BB2" s="88"/>
+      <c r="BC2" s="88"/>
+      <c r="BD2" s="88"/>
+      <c r="BE2" s="88"/>
+      <c r="BF2" s="88"/>
+      <c r="BG2" s="88"/>
+      <c r="BH2" s="88"/>
+      <c r="BI2" s="88"/>
+      <c r="BJ2" s="88"/>
+      <c r="BK2" s="88"/>
+      <c r="BL2" s="89"/>
     </row>
     <row r="3" spans="1:64" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A3" s="2"/>
@@ -2875,7 +5011,7 @@
         <v/>
       </c>
       <c r="AK10" s="45" t="str">
-        <f t="shared" ref="AK10:BP10" si="2">IF(AND(AK7&lt;&gt;0,AK9&lt;AK7),AK14/(AK7-AK9),IF(AND(AK7&lt;&gt;0,AK9&gt;=AK7),0,""))</f>
+        <f t="shared" ref="AK10:BL10" si="2">IF(AND(AK7&lt;&gt;0,AK9&lt;AK7),AK14/(AK7-AK9),IF(AND(AK7&lt;&gt;0,AK9&gt;=AK7),0,""))</f>
         <v/>
       </c>
       <c r="AL10" s="45" t="str">
@@ -4145,7 +6281,7 @@
     <row r="23" spans="1:64" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A23" s="2"/>
       <c r="B23" s="72"/>
-      <c r="C23" s="89"/>
+      <c r="C23" s="90"/>
       <c r="D23" s="76" t="s">
         <v>74</v>
       </c>
@@ -4333,7 +6469,7 @@
     <row r="24" spans="1:64" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" s="2"/>
       <c r="B24" s="72"/>
-      <c r="C24" s="90"/>
+      <c r="C24" s="91"/>
       <c r="D24" s="79" t="s">
         <v>75</v>
       </c>
@@ -4521,7 +6657,7 @@
     <row r="25" spans="1:64" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A25" s="2"/>
       <c r="B25" s="72"/>
-      <c r="C25" s="89"/>
+      <c r="C25" s="90"/>
       <c r="D25" s="76" t="s">
         <v>74</v>
       </c>
@@ -4708,7 +6844,7 @@
     </row>
     <row r="26" spans="1:64" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A26" s="2"/>
-      <c r="C26" s="90"/>
+      <c r="C26" s="91"/>
       <c r="D26" s="79" t="s">
         <v>75</v>
       </c>
@@ -4896,7 +7032,7 @@
     <row r="27" spans="1:64" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A27" s="2"/>
       <c r="B27" s="72"/>
-      <c r="C27" s="89"/>
+      <c r="C27" s="90"/>
       <c r="D27" s="76" t="s">
         <v>74</v>
       </c>
@@ -5084,7 +7220,7 @@
     <row r="28" spans="1:64" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A28" s="2"/>
       <c r="B28" s="72"/>
-      <c r="C28" s="90"/>
+      <c r="C28" s="91"/>
       <c r="D28" s="79" t="s">
         <v>75</v>
       </c>
@@ -5272,7 +7408,7 @@
     <row r="29" spans="1:64" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A29" s="2"/>
       <c r="B29" s="72"/>
-      <c r="C29" s="89"/>
+      <c r="C29" s="90"/>
       <c r="D29" s="76" t="s">
         <v>74</v>
       </c>
@@ -5460,7 +7596,7 @@
     <row r="30" spans="1:64" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A30" s="2"/>
       <c r="B30" s="72"/>
-      <c r="C30" s="90"/>
+      <c r="C30" s="91"/>
       <c r="D30" s="79" t="s">
         <v>75</v>
       </c>
@@ -5648,7 +7784,7 @@
     <row r="31" spans="1:64" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A31" s="2"/>
       <c r="B31" s="72"/>
-      <c r="C31" s="89"/>
+      <c r="C31" s="90"/>
       <c r="D31" s="76" t="s">
         <v>74</v>
       </c>
@@ -5836,7 +7972,7 @@
     <row r="32" spans="1:64" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A32" s="2"/>
       <c r="B32" s="72"/>
-      <c r="C32" s="90"/>
+      <c r="C32" s="91"/>
       <c r="D32" s="79" t="s">
         <v>75</v>
       </c>
@@ -6024,7 +8160,7 @@
     <row r="33" spans="1:64" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A33" s="2"/>
       <c r="B33" s="72"/>
-      <c r="C33" s="89"/>
+      <c r="C33" s="90"/>
       <c r="D33" s="76" t="s">
         <v>74</v>
       </c>
@@ -6212,7 +8348,7 @@
     <row r="34" spans="1:64" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A34" s="2"/>
       <c r="B34" s="72"/>
-      <c r="C34" s="90"/>
+      <c r="C34" s="91"/>
       <c r="D34" s="79" t="s">
         <v>75</v>
       </c>
@@ -6400,7 +8536,7 @@
     <row r="35" spans="1:64" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A35" s="2"/>
       <c r="B35" s="72"/>
-      <c r="C35" s="89"/>
+      <c r="C35" s="90"/>
       <c r="D35" s="76" t="s">
         <v>74</v>
       </c>
@@ -6588,7 +8724,7 @@
     <row r="36" spans="1:64" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A36" s="2"/>
       <c r="B36" s="72"/>
-      <c r="C36" s="90"/>
+      <c r="C36" s="91"/>
       <c r="D36" s="79" t="s">
         <v>75</v>
       </c>
@@ -6776,7 +8912,7 @@
     <row r="37" spans="1:64" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A37" s="2"/>
       <c r="B37" s="72"/>
-      <c r="C37" s="89"/>
+      <c r="C37" s="90"/>
       <c r="D37" s="76" t="s">
         <v>74</v>
       </c>
@@ -6964,7 +9100,7 @@
     <row r="38" spans="1:64" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A38" s="2"/>
       <c r="B38" s="72"/>
-      <c r="C38" s="90"/>
+      <c r="C38" s="91"/>
       <c r="D38" s="79" t="s">
         <v>75</v>
       </c>
@@ -7152,7 +9288,7 @@
     <row r="39" spans="1:64" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A39" s="2"/>
       <c r="B39" s="72"/>
-      <c r="C39" s="89"/>
+      <c r="C39" s="90"/>
       <c r="D39" s="76" t="s">
         <v>74</v>
       </c>
@@ -7340,7 +9476,7 @@
     <row r="40" spans="1:64" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A40" s="2"/>
       <c r="B40" s="72"/>
-      <c r="C40" s="90"/>
+      <c r="C40" s="91"/>
       <c r="D40" s="79" t="s">
         <v>75</v>
       </c>
@@ -7528,7 +9664,7 @@
     <row r="41" spans="1:64" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A41" s="2"/>
       <c r="B41" s="72"/>
-      <c r="C41" s="91"/>
+      <c r="C41" s="92"/>
       <c r="D41" s="76" t="s">
         <v>74</v>
       </c>
@@ -7716,7 +9852,7 @@
     <row r="42" spans="1:64" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A42" s="2"/>
       <c r="B42" s="72"/>
-      <c r="C42" s="92"/>
+      <c r="C42" s="93"/>
       <c r="D42" s="79" t="s">
         <v>75</v>
       </c>
@@ -8462,11 +10598,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="AO2:AZ2"/>
-    <mergeCell ref="BA2:BL2"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="C39:C40"/>
     <mergeCell ref="C41:C42"/>
     <mergeCell ref="AC2:AN2"/>
     <mergeCell ref="C25:C26"/>
@@ -8478,6 +10609,11 @@
     <mergeCell ref="E2:P2"/>
     <mergeCell ref="Q2:AB2"/>
     <mergeCell ref="C23:C24"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="AO2:AZ2"/>
+    <mergeCell ref="BA2:BL2"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C39:C40"/>
   </mergeCells>
   <conditionalFormatting sqref="E21:BL21">
     <cfRule type="cellIs" dxfId="1" priority="6" operator="lessThan">

</xml_diff>